<commit_message>
Pruebas de tiempo 1
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 4.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/2025-10/Laboratorios/Lab 04 - Pilas y colas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aef29e720c6d702c/Desktop/UNIANDES/Trabajos/Pregrado/Segundo Semestre/EDA/Laboratorio4-G03/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{059725CA-9D74-4145-8FC3-28FE5756BBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CAB1D75-7132-4A69-A395-BC4C20E1FCBD}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{059725CA-9D74-4145-8FC3-28FE5756BBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E759D55D-126D-4459-A3DA-AB2472036876}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Data Lab 4" sheetId="1" r:id="rId1"/>
@@ -293,139 +293,6 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -567,6 +434,139 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -8396,19 +8396,19 @@
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tamaño de la muestra (ARRAY_LIST)" dataDxfId="16">
       <calculatedColumnFormula>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="enqueue (Array List) " dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="dequeue (Array List) " dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="peek (Array List) " dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{092BA754-1EE8-42B8-A0C9-8E5FBAFE3FD2}" name="push (Array List)" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{F7FD567A-4A42-4CDC-9449-A0BA8E9714D3}" name="pop (Array List)" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{91D17C3E-2CFC-4978-91FF-19ADDF3A1CD9}" name="top(Array List) " dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="enqueue (Array List) " dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="dequeue (Array List) " dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="peek (Array List) " dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{092BA754-1EE8-42B8-A0C9-8E5FBAFE3FD2}" name="push (Array List)" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{F7FD567A-4A42-4CDC-9449-A0BA8E9714D3}" name="pop (Array List)" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{91D17C3E-2CFC-4978-91FF-19ADDF3A1CD9}" name="top(Array List) " dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A13:H21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A13:H21" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A13:H21" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -8420,13 +8420,13 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Porcentaje de la muestra [pct]" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Porcentaje de la muestra [pct]" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="6">
       <calculatedColumnFormula>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="enqueue (Linked List) " dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="dequeue (Linked List)  " dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="peek (Linked List)  " dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="enqueue (Linked List) " dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="dequeue (Linked List)  " dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="peek (Linked List)  " dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{D4319BDE-1663-4E02-A459-D4E464B40376}" name="push (Linked List) " dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{D1102AA4-3669-4976-AB80-8CA1D8EED93A}" name="pop (Linked List) " dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{A75BD949-6BC0-4683-B105-18DE72DE82D5}" name="top(Linked List) " dataDxfId="0"/>
@@ -8735,16 +8735,16 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="6" customWidth="1"/>
-    <col min="6" max="12" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" style="6" customWidth="1"/>
+    <col min="6" max="12" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" customHeight="1">
@@ -8759,7 +8759,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="30">
+    <row r="2" spans="1:8" s="5" customFormat="1" ht="28">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="14">
       <c r="A3" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -8800,7 +8800,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1">
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="14">
       <c r="A4" s="2">
         <v>0.05</v>
       </c>
@@ -8917,7 +8917,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="30">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="28">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -8943,7 +8943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="14">
       <c r="A14" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -8958,7 +8958,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="14">
       <c r="A15" s="2">
         <v>0.05</v>
       </c>
@@ -9080,116 +9080,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
-      <UserInfo>
-        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Arturo Henao Chaparro</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Carlos Marin Morales</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sofia Duque Gomez</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Andres Felipe Romero Brand</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
-        <AccountId>92</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan David Diaz Ipuz</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Isaac David Bermudez Lara</DisplayName>
-        <AccountId>95</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
-        <AccountId>97</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kevin Cohen Solano</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
-        <AccountId>96</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9442,27 +9338,122 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
+      <UserInfo>
+        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Arturo Henao Chaparro</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Carlos Marin Morales</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sofia Duque Gomez</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Andres Felipe Romero Brand</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
+        <AccountId>92</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan David Diaz Ipuz</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Isaac David Bermudez Lara</DisplayName>
+        <AccountId>95</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
+        <AccountId>97</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kevin Cohen Solano</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
+        <AccountId>96</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9487,9 +9478,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>